<commit_message>
Added more diagrams Added poster as pdf
</commit_message>
<xml_diff>
--- a/Poster/diagram.xlsx
+++ b/Poster/diagram.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projekte\Universität\SW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projekte\Universität\SW\Poster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D28992E-293B-4678-BE38-FA345224279F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA70646-6821-488A-8950-B86B6EE5A943}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Jahr</t>
   </si>
@@ -77,6 +77,24 @@
   </si>
   <si>
     <t>CDU/CSU</t>
+  </si>
+  <si>
+    <t>Kernenergie</t>
+  </si>
+  <si>
+    <t>Braunkohle</t>
+  </si>
+  <si>
+    <t>Steinkohle</t>
+  </si>
+  <si>
+    <t>Öl</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Pumpspeicher Erzeugung</t>
   </si>
 </sst>
 </file>
@@ -2229,6 +2247,2000 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Wasserkraft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$N$2:$N$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>20.745000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.638000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.030999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.443000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.030999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.952999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.670999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.210999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.844999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19.41</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18.812000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20.66</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20.079000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17.140999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.137</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18.402000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-6A2D-48C3-B900-6BB30B5ABB25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Biomasse</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$O$2:$O$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>8.3849999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.224</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.212</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.43</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.783999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31.324999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34.061999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39.951999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41.042999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42.640999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44.151000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44.680999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44.792000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45.805</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43.71</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>47.148000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-6A2D-48C3-B900-6BB30B5ABB25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kernenergie</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$P$2:$P$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>158.37799999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>154.61199999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>158.71100000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>133.22900000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>140.71</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>127.69</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>132.971</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>102.241</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>94.18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>92.126999999999995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>91.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>86.765000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>80.037999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>72.155000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>71.866</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70.992000000000004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>60.917000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-6A2D-48C3-B900-6BB30B5ABB25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Braunkohle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$Q$2:$Q$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>142.136</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>138.20500000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>135.08699999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>138.565</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>134.49799999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>130.99199999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>130.429</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>134.05600000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>141.86799999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>145.12200000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>140.791</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>139.37100000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>134.886</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>133.983</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>131.49799999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>101.92400000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>82.128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-6A2D-48C3-B900-6BB30B5ABB25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Steinkohle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$R$2:$R$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>116.64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>112.973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>116.47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>119.131</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105.714</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91.653999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99.706000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>96.498999999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>105.83</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>110.724</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>107.73399999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>106.208</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>99.765000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>81.724000000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>72.406000000000006</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>49.503</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>35.591000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-6A2D-48C3-B900-6BB30B5ABB25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Öl</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$S$2:$S$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1.8740000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4009999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0859999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.234</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2109999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.492</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.544</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.153</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.872</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.90400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0549999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0409999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.78200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.745</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-6A2D-48C3-B900-6BB30B5ABB25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$T$2:$T$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>44.881999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52.31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54.957999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56.256999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66.936999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57.598999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>63.091000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59.761000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>49.868000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39.584000000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31.122</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30.123000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>46.503</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>48.956000000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44.533000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>52.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>56.767000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-6A2D-48C3-B900-6BB30B5ABB25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$U$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Andere</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$U$2:$U$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>10.581</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.260999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.486000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.59</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.987</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.9800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.532</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.8310000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.0149999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.8369999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.7669999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.6920000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.9830000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.83</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.6080000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.6080000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-6A2D-48C3-B900-6BB30B5ABB25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$V$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pumpspeicher Erzeugung</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$V$2:$V$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.077</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.9860000000000007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.2469999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.058</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.9529999999999994</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.57</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-6A2D-48C3-B900-6BB30B5ABB25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$W$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Wind</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$W$2:$W$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>26.018999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.774000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.324000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.506999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41.384999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39.42</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38.546999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>49.856999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>51.68</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52.737000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>58.497</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>80.623999999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>79.924000000000007</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>105.693</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>109.95099999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>125.89400000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>131.851</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-6A2D-48C3-B900-6BB30B5ABB25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$X$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Solar</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2020</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$X$2:$X$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.55700000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.282</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0750000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.5830000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.728999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.599</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26.38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31.01</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>36.055999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>38.725999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>38.097999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39.401000000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45.783999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>46.392000000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>51.418999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000012-6A2D-48C3-B900-6BB30B5ABB25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="212835296"/>
+        <c:axId val="212836128"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="212835296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Jahr</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="212836128"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="212836128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Terawatt</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="212835296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="2800"/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2270,6 +4282,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3330,20 +5382,525 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>71437</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>166688</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>504392</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>149370</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>57</xdr:col>
-      <xdr:colOff>362790</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>175093</xdr:rowOff>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>189609</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>157775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3370,16 +5927,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>375729</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>427684</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>29327</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3399,6 +5956,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>329046</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>152060</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F079428A-F8D2-415A-8E0B-16FC4E455796}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3670,10 +6265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA38" sqref="AA38"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3686,9 +6281,11 @@
     <col min="7" max="7" width="9.85546875" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="2"/>
     <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3726,8 +6323,41 @@
         <v>9</v>
       </c>
       <c r="M1" s="8"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" t="s">
+        <v>8</v>
+      </c>
+      <c r="V1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" t="s">
+        <v>6</v>
+      </c>
+      <c r="X1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>2004</v>
       </c>
@@ -3750,8 +6380,41 @@
         <v>6.2</v>
       </c>
       <c r="H2"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>20.745000000000001</v>
+      </c>
+      <c r="O2">
+        <v>8.3849999999999998</v>
+      </c>
+      <c r="P2">
+        <v>158.37799999999999</v>
+      </c>
+      <c r="Q2">
+        <v>142.136</v>
+      </c>
+      <c r="R2">
+        <v>116.64</v>
+      </c>
+      <c r="S2">
+        <v>1.8740000000000001</v>
+      </c>
+      <c r="T2">
+        <v>44.881999999999998</v>
+      </c>
+      <c r="U2">
+        <v>10.581</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>26.018999999999998</v>
+      </c>
+      <c r="X2">
+        <v>0.55700000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2005</v>
       </c>
@@ -3788,8 +6451,41 @@
       <c r="L3">
         <v>1910</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>19.638000000000002</v>
+      </c>
+      <c r="O3">
+        <v>11.61</v>
+      </c>
+      <c r="P3">
+        <v>154.61199999999999</v>
+      </c>
+      <c r="Q3">
+        <v>138.20500000000001</v>
+      </c>
+      <c r="R3">
+        <v>112.973</v>
+      </c>
+      <c r="S3">
+        <v>2.4009999999999998</v>
+      </c>
+      <c r="T3">
+        <v>52.31</v>
+      </c>
+      <c r="U3">
+        <v>12.260999999999999</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>27.774000000000001</v>
+      </c>
+      <c r="X3">
+        <v>1.282</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2006</v>
       </c>
@@ -3826,8 +6522,41 @@
       <c r="L4">
         <v>2270</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>20.030999999999999</v>
+      </c>
+      <c r="O4">
+        <v>15.224</v>
+      </c>
+      <c r="P4">
+        <v>158.71100000000001</v>
+      </c>
+      <c r="Q4">
+        <v>135.08699999999999</v>
+      </c>
+      <c r="R4">
+        <v>116.47</v>
+      </c>
+      <c r="S4">
+        <v>2.0859999999999999</v>
+      </c>
+      <c r="T4">
+        <v>54.957999999999998</v>
+      </c>
+      <c r="U4">
+        <v>12.486000000000001</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>31.324000000000002</v>
+      </c>
+      <c r="X4">
+        <v>2.2200000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2007</v>
       </c>
@@ -3864,8 +6593,41 @@
       <c r="L5">
         <v>2280</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>21.17</v>
+      </c>
+      <c r="O5">
+        <v>20.212</v>
+      </c>
+      <c r="P5">
+        <v>133.22900000000001</v>
+      </c>
+      <c r="Q5">
+        <v>138.565</v>
+      </c>
+      <c r="R5">
+        <v>119.131</v>
+      </c>
+      <c r="S5">
+        <v>2.234</v>
+      </c>
+      <c r="T5">
+        <v>56.256999999999998</v>
+      </c>
+      <c r="U5">
+        <v>12.59</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>40.506999999999998</v>
+      </c>
+      <c r="X5">
+        <v>3.0750000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2008</v>
       </c>
@@ -3902,8 +6664,41 @@
       <c r="L6">
         <v>1980</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>20.443000000000001</v>
+      </c>
+      <c r="O6">
+        <v>23.43</v>
+      </c>
+      <c r="P6">
+        <v>140.71</v>
+      </c>
+      <c r="Q6">
+        <v>134.49799999999999</v>
+      </c>
+      <c r="R6">
+        <v>105.714</v>
+      </c>
+      <c r="S6">
+        <v>2.2109999999999999</v>
+      </c>
+      <c r="T6">
+        <v>66.936999999999998</v>
+      </c>
+      <c r="U6">
+        <v>12.987</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>41.384999999999998</v>
+      </c>
+      <c r="X6">
+        <v>4.42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2009</v>
       </c>
@@ -3940,8 +6735,41 @@
       <c r="L7">
         <v>2020</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>19.030999999999999</v>
+      </c>
+      <c r="O7">
+        <v>28.783999999999999</v>
+      </c>
+      <c r="P7">
+        <v>127.69</v>
+      </c>
+      <c r="Q7">
+        <v>130.99199999999999</v>
+      </c>
+      <c r="R7">
+        <v>91.653999999999996</v>
+      </c>
+      <c r="S7">
+        <v>2.492</v>
+      </c>
+      <c r="T7">
+        <v>57.598999999999997</v>
+      </c>
+      <c r="U7">
+        <v>4.51</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>39.42</v>
+      </c>
+      <c r="X7">
+        <v>6.5830000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>2010</v>
       </c>
@@ -3978,8 +6806,41 @@
       <c r="L8">
         <v>2240</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>20.952999999999999</v>
+      </c>
+      <c r="O8">
+        <v>31.324999999999999</v>
+      </c>
+      <c r="P8">
+        <v>132.971</v>
+      </c>
+      <c r="Q8">
+        <v>130.429</v>
+      </c>
+      <c r="R8">
+        <v>99.706000000000003</v>
+      </c>
+      <c r="S8">
+        <v>2.544</v>
+      </c>
+      <c r="T8">
+        <v>63.091000000000001</v>
+      </c>
+      <c r="U8">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>38.546999999999997</v>
+      </c>
+      <c r="X8">
+        <v>11.728999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>2011</v>
       </c>
@@ -4016,8 +6877,41 @@
       <c r="L9">
         <v>3120</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>17.670999999999999</v>
+      </c>
+      <c r="O9">
+        <v>34.061999999999998</v>
+      </c>
+      <c r="P9">
+        <v>102.241</v>
+      </c>
+      <c r="Q9">
+        <v>134.05600000000001</v>
+      </c>
+      <c r="R9">
+        <v>96.498999999999995</v>
+      </c>
+      <c r="S9">
+        <v>1.6379999999999999</v>
+      </c>
+      <c r="T9">
+        <v>59.761000000000003</v>
+      </c>
+      <c r="U9">
+        <v>4.532</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>49.856999999999999</v>
+      </c>
+      <c r="X9">
+        <v>19.599</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>2012</v>
       </c>
@@ -4054,8 +6948,41 @@
       <c r="L10">
         <v>790</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>21.210999999999999</v>
+      </c>
+      <c r="O10">
+        <v>39.951999999999998</v>
+      </c>
+      <c r="P10">
+        <v>94.18</v>
+      </c>
+      <c r="Q10">
+        <v>141.86799999999999</v>
+      </c>
+      <c r="R10">
+        <v>105.83</v>
+      </c>
+      <c r="S10">
+        <v>2.153</v>
+      </c>
+      <c r="T10">
+        <v>49.868000000000002</v>
+      </c>
+      <c r="U10">
+        <v>4.8310000000000004</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>51.68</v>
+      </c>
+      <c r="X10">
+        <v>26.38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>2013</v>
       </c>
@@ -4092,8 +7019,41 @@
       <c r="L11">
         <v>700</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>22.844999999999999</v>
+      </c>
+      <c r="O11">
+        <v>41.042999999999999</v>
+      </c>
+      <c r="P11">
+        <v>92.126999999999995</v>
+      </c>
+      <c r="Q11">
+        <v>145.12200000000001</v>
+      </c>
+      <c r="R11">
+        <v>110.724</v>
+      </c>
+      <c r="S11">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="T11">
+        <v>39.584000000000003</v>
+      </c>
+      <c r="U11">
+        <v>6.0149999999999997</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>52.737000000000002</v>
+      </c>
+      <c r="X11">
+        <v>31.01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>2014</v>
       </c>
@@ -4130,8 +7090,41 @@
       <c r="L12">
         <v>670</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>19.41</v>
+      </c>
+      <c r="O12">
+        <v>42.640999999999998</v>
+      </c>
+      <c r="P12">
+        <v>91.8</v>
+      </c>
+      <c r="Q12">
+        <v>140.791</v>
+      </c>
+      <c r="R12">
+        <v>107.73399999999999</v>
+      </c>
+      <c r="S12">
+        <v>0.872</v>
+      </c>
+      <c r="T12">
+        <v>31.122</v>
+      </c>
+      <c r="U12">
+        <v>4.8369999999999997</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>58.497</v>
+      </c>
+      <c r="X12">
+        <v>36.055999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>2015</v>
       </c>
@@ -4168,8 +7161,41 @@
       <c r="L13">
         <v>220</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>18.812000000000001</v>
+      </c>
+      <c r="O13">
+        <v>44.151000000000003</v>
+      </c>
+      <c r="P13">
+        <v>86.765000000000001</v>
+      </c>
+      <c r="Q13">
+        <v>139.37100000000001</v>
+      </c>
+      <c r="R13">
+        <v>106.208</v>
+      </c>
+      <c r="S13">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="T13">
+        <v>30.123000000000001</v>
+      </c>
+      <c r="U13">
+        <v>2.7669999999999999</v>
+      </c>
+      <c r="V13">
+        <v>9.077</v>
+      </c>
+      <c r="W13">
+        <v>80.623999999999995</v>
+      </c>
+      <c r="X13">
+        <v>38.725999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>2016</v>
       </c>
@@ -4206,8 +7232,41 @@
       <c r="L14">
         <v>270</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>20.66</v>
+      </c>
+      <c r="O14">
+        <v>44.680999999999997</v>
+      </c>
+      <c r="P14">
+        <v>80.037999999999997</v>
+      </c>
+      <c r="Q14">
+        <v>134.886</v>
+      </c>
+      <c r="R14">
+        <v>99.765000000000001</v>
+      </c>
+      <c r="S14">
+        <v>1.0549999999999999</v>
+      </c>
+      <c r="T14">
+        <v>46.503</v>
+      </c>
+      <c r="U14">
+        <v>2.6920000000000002</v>
+      </c>
+      <c r="V14">
+        <v>8.9860000000000007</v>
+      </c>
+      <c r="W14">
+        <v>79.924000000000007</v>
+      </c>
+      <c r="X14">
+        <v>38.097999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>2017</v>
       </c>
@@ -4244,8 +7303,41 @@
       <c r="L15">
         <v>280</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>20.079000000000001</v>
+      </c>
+      <c r="O15">
+        <v>44.792000000000002</v>
+      </c>
+      <c r="P15">
+        <v>72.155000000000001</v>
+      </c>
+      <c r="Q15">
+        <v>133.983</v>
+      </c>
+      <c r="R15">
+        <v>81.724000000000004</v>
+      </c>
+      <c r="S15">
+        <v>1.0409999999999999</v>
+      </c>
+      <c r="T15">
+        <v>48.956000000000003</v>
+      </c>
+      <c r="U15">
+        <v>1.9830000000000001</v>
+      </c>
+      <c r="V15">
+        <v>9.2469999999999999</v>
+      </c>
+      <c r="W15">
+        <v>105.693</v>
+      </c>
+      <c r="X15">
+        <v>39.401000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>2018</v>
       </c>
@@ -4282,8 +7374,41 @@
       <c r="L16">
         <v>390</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <v>17.140999999999998</v>
+      </c>
+      <c r="O16">
+        <v>45.805</v>
+      </c>
+      <c r="P16">
+        <v>71.866</v>
+      </c>
+      <c r="Q16">
+        <v>131.49799999999999</v>
+      </c>
+      <c r="R16">
+        <v>72.406000000000006</v>
+      </c>
+      <c r="S16">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="T16">
+        <v>44.533000000000001</v>
+      </c>
+      <c r="U16">
+        <v>2.83</v>
+      </c>
+      <c r="V16">
+        <v>10.058</v>
+      </c>
+      <c r="W16">
+        <v>109.95099999999999</v>
+      </c>
+      <c r="X16">
+        <v>45.783999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>2019</v>
       </c>
@@ -4320,8 +7445,41 @@
       <c r="L17">
         <v>390</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>20.137</v>
+      </c>
+      <c r="O17">
+        <v>43.71</v>
+      </c>
+      <c r="P17">
+        <v>70.992000000000004</v>
+      </c>
+      <c r="Q17">
+        <v>101.92400000000001</v>
+      </c>
+      <c r="R17">
+        <v>49.503</v>
+      </c>
+      <c r="S17">
+        <v>0.745</v>
+      </c>
+      <c r="T17">
+        <v>52.9</v>
+      </c>
+      <c r="U17">
+        <v>2.6080000000000001</v>
+      </c>
+      <c r="V17">
+        <v>8.9529999999999994</v>
+      </c>
+      <c r="W17">
+        <v>125.89400000000001</v>
+      </c>
+      <c r="X17">
+        <v>46.392000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>2020</v>
       </c>
@@ -4357,6 +7515,39 @@
       </c>
       <c r="L18">
         <v>420</v>
+      </c>
+      <c r="N18">
+        <v>18.402000000000001</v>
+      </c>
+      <c r="O18">
+        <v>47.148000000000003</v>
+      </c>
+      <c r="P18">
+        <v>60.917000000000002</v>
+      </c>
+      <c r="Q18">
+        <v>82.128</v>
+      </c>
+      <c r="R18">
+        <v>35.591000000000001</v>
+      </c>
+      <c r="S18">
+        <v>0.59</v>
+      </c>
+      <c r="T18">
+        <v>56.767000000000003</v>
+      </c>
+      <c r="U18">
+        <v>2.6080000000000001</v>
+      </c>
+      <c r="V18">
+        <v>10.57</v>
+      </c>
+      <c r="W18">
+        <v>131.851</v>
+      </c>
+      <c r="X18">
+        <v>51.418999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -4371,7 +7562,7 @@
   <dimension ref="A1:P530"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:O18"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>